<commit_message>
working now we need this on the chatgpt
</commit_message>
<xml_diff>
--- a/cotizacion/cotizacion.xlsx
+++ b/cotizacion/cotizacion.xlsx
@@ -236,7 +236,6 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">NOTA 3</t>
     </r>
@@ -246,9 +245,8 @@
         <color rgb="FF000000"/>
         <rFont val="Arial Narrow"/>
         <family val="2"/>
-        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">:El servicio incluye monitoreo en tiempo real a través de app para celular.</t>
+      <t xml:space="preserve">:El servicio incluye una app para que pueda hacer monitoreo en tiempo real a través de celular.</t>
     </r>
   </si>
   <si>
@@ -306,7 +304,7 @@
     <numFmt numFmtId="171" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="172" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="41">
+  <fonts count="43">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -450,6 +448,19 @@
       <name val="Arial Narrow"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -995,7 +1006,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1015,11 +1026,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1031,11 +1042,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="172" fontId="23" fillId="0" borderId="4" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="172" fontId="25" fillId="0" borderId="4" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1043,7 +1054,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1055,19 +1066,19 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="24" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="26" fillId="0" borderId="0" xfId="17" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1075,130 +1086,130 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="171" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="171" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="fill" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="34" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="172" fontId="34" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="172" fontId="36" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="172" fontId="34" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="172" fontId="32" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="38" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1207,59 +1218,59 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="40" fillId="0" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="42" fillId="0" borderId="0" xfId="25" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1353,9 +1364,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>674280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>314</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1369,7 +1380,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="57903120"/>
-          <a:ext cx="10149120" cy="346320"/>
+          <a:ext cx="10148760" cy="345960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1390,9 +1401,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>674280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>362</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1406,7 +1417,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="66780360"/>
-          <a:ext cx="10149120" cy="346680"/>
+          <a:ext cx="10148760" cy="346320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1427,9 +1438,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>674280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>410</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1443,7 +1454,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="75638880"/>
-          <a:ext cx="10149120" cy="346320"/>
+          <a:ext cx="10148760" cy="345960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1464,9 +1475,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>674280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>458</xdr:row>
-      <xdr:rowOff>261360</xdr:rowOff>
+      <xdr:rowOff>261000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1480,7 +1491,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1564560" y="84430440"/>
-          <a:ext cx="10149120" cy="346320"/>
+          <a:ext cx="10148760" cy="345960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1501,9 +1512,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>680400</xdr:colOff>
+      <xdr:colOff>680040</xdr:colOff>
       <xdr:row>122</xdr:row>
-      <xdr:rowOff>326160</xdr:rowOff>
+      <xdr:rowOff>325800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1517,7 +1528,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="22307400"/>
-          <a:ext cx="1453680" cy="497880"/>
+          <a:ext cx="1453320" cy="497520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1538,9 +1549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>680400</xdr:colOff>
+      <xdr:colOff>680040</xdr:colOff>
       <xdr:row>170</xdr:row>
-      <xdr:rowOff>326160</xdr:rowOff>
+      <xdr:rowOff>325800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1554,7 +1565,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="31204080"/>
-          <a:ext cx="1453680" cy="497520"/>
+          <a:ext cx="1453320" cy="497160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1575,9 +1586,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>680400</xdr:colOff>
+      <xdr:colOff>680040</xdr:colOff>
       <xdr:row>218</xdr:row>
-      <xdr:rowOff>326160</xdr:rowOff>
+      <xdr:rowOff>325800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1591,7 +1602,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="40081320"/>
-          <a:ext cx="1453680" cy="497520"/>
+          <a:ext cx="1453320" cy="497160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1612,9 +1623,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>680400</xdr:colOff>
+      <xdr:colOff>680040</xdr:colOff>
       <xdr:row>266</xdr:row>
-      <xdr:rowOff>326160</xdr:rowOff>
+      <xdr:rowOff>325800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1628,7 +1639,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1148760" y="48967920"/>
-          <a:ext cx="1453680" cy="497880"/>
+          <a:ext cx="1453320" cy="497520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1651,7 +1662,7 @@
   <dimension ref="B2:O505"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K52" activeCellId="0" sqref="K52"/>
+      <selection pane="topLeft" activeCell="F48" activeCellId="0" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.62890625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>